<commit_message>
Finalizada documentación, menos SA
</commit_message>
<xml_diff>
--- a/data/Iteracion2/Modelo Relacional.xlsx
+++ b/data/Iteracion2/Modelo Relacional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estudiante\Pictures\Sistrans\Sistrans-D01\data\Iteracion2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4D121B69-2588-44AC-B9EA-0D037EED0676}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FA519FB2-D6BF-41AC-BE1B-BEF8BCEFBFF8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="121">
   <si>
     <t>PRODUCTO</t>
   </si>
@@ -385,6 +385,9 @@
   </si>
   <si>
     <t>PK, FK_TIPO.nombre, UA</t>
+  </si>
+  <si>
+    <t>codigoBarrasProducto</t>
   </si>
 </sst>
 </file>
@@ -622,30 +625,6 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -658,12 +637,21 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="11" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="11" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -673,9 +661,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -686,6 +671,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -985,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6:R6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,23 +1013,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -1123,19 +1126,19 @@
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="32"/>
-      <c r="H6" s="19" t="s">
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="27"/>
+      <c r="H6" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
       <c r="M6" s="13" t="s">
         <v>2</v>
       </c>
@@ -1173,7 +1176,7 @@
         <v>29</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>3</v>
@@ -1230,27 +1233,27 @@
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="32"/>
-      <c r="H10" s="30" t="s">
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="27"/>
+      <c r="H10" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="31"/>
-      <c r="J10" s="32"/>
-      <c r="L10" s="23" t="s">
+      <c r="I10" s="26"/>
+      <c r="J10" s="27"/>
+      <c r="L10" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="M10" s="23"/>
-      <c r="O10" s="23" t="s">
+      <c r="M10" s="21"/>
+      <c r="O10" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
@@ -1275,7 +1278,7 @@
         <v>28</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>20</v>
@@ -1335,14 +1338,14 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="32"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="27"/>
       <c r="J14" s="13" t="s">
         <v>62</v>
       </c>
@@ -1429,18 +1432,18 @@
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="E18" s="35" t="s">
+      <c r="C18" s="28"/>
+      <c r="E18" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="37"/>
-      <c r="H18" s="19" t="s">
+      <c r="F18" s="31"/>
+      <c r="H18" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="I18" s="19"/>
+      <c r="I18" s="24"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
@@ -1458,8 +1461,8 @@
       <c r="H19" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="I19" s="6" t="s">
-        <v>74</v>
+      <c r="I19" s="5" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
@@ -1483,21 +1486,21 @@
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="37"/>
-      <c r="I22" s="16" t="s">
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="31"/>
+      <c r="I22" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="18"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="34"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
@@ -1570,20 +1573,20 @@
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="21"/>
-      <c r="D26" s="22"/>
-      <c r="I26" s="28" t="s">
+      <c r="C26" s="36"/>
+      <c r="D26" s="37"/>
+      <c r="I26" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="29"/>
-      <c r="M26" s="29"/>
-      <c r="N26" s="29"/>
-      <c r="O26" s="29"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
@@ -1650,17 +1653,17 @@
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="33" t="s">
+      <c r="B30" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
@@ -1721,15 +1724,15 @@
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="24" t="s">
+      <c r="B34" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="F34" s="26" t="s">
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="F34" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="G34" s="27"/>
+      <c r="G34" s="19"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
@@ -1767,6 +1770,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="B30:J30"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="I26:O26"/>
     <mergeCell ref="H6:K6"/>
@@ -1780,12 +1789,6 @@
     <mergeCell ref="B22:G22"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="I22:M22"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="B30:J30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Un MONTON de documentación. Carrito de compras implementado completamente.
</commit_message>
<xml_diff>
--- a/data/Iteracion2/Modelo Relacional.xlsx
+++ b/data/Iteracion2/Modelo Relacional.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estudiante\Pictures\Sistrans\Sistrans-D01\data\Iteracion2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Universidad\4toSemestre\Sistrans\Iteraciones\Iteración2\Proyecto eclipse\Sistrans-D01\data\Iteracion2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FA519FB2-D6BF-41AC-BE1B-BEF8BCEFBFF8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="123">
   <si>
     <t>PRODUCTO</t>
   </si>
@@ -388,13 +387,19 @@
   </si>
   <si>
     <t>codigoBarrasProducto</t>
+  </si>
+  <si>
+    <t>estaEnPromocion</t>
+  </si>
+  <si>
+    <t>UA, NN, CK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -410,14 +415,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -625,6 +622,57 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -640,58 +688,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -985,11 +982,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,23 +1010,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -1077,6 +1075,9 @@
       <c r="P3" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="Q3" s="1" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
@@ -1124,21 +1125,24 @@
       <c r="P4" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="Q4" s="3" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="27"/>
-      <c r="H6" s="24" t="s">
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="22"/>
+      <c r="H6" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
       <c r="M6" s="13" t="s">
         <v>2</v>
       </c>
@@ -1233,27 +1237,27 @@
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="27"/>
-      <c r="H10" s="25" t="s">
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="22"/>
+      <c r="H10" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="26"/>
-      <c r="J10" s="27"/>
-      <c r="L10" s="21" t="s">
+      <c r="I10" s="21"/>
+      <c r="J10" s="22"/>
+      <c r="L10" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="M10" s="21"/>
-      <c r="O10" s="21" t="s">
+      <c r="M10" s="19"/>
+      <c r="O10" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
@@ -1292,8 +1296,8 @@
       <c r="P11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q11" s="1" t="s">
-        <v>1</v>
+      <c r="Q11" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
@@ -1338,14 +1342,14 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="27"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="22"/>
       <c r="J14" s="13" t="s">
         <v>62</v>
       </c>
@@ -1432,18 +1436,18 @@
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="E18" s="29" t="s">
+      <c r="C18" s="23"/>
+      <c r="E18" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="31"/>
-      <c r="H18" s="24" t="s">
+      <c r="F18" s="26"/>
+      <c r="H18" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="I18" s="24"/>
+      <c r="I18" s="18"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
@@ -1486,21 +1490,21 @@
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="31"/>
-      <c r="I22" s="32" t="s">
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="26"/>
+      <c r="I22" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="34"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="29"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
@@ -1573,20 +1577,20 @@
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="37"/>
-      <c r="I26" s="22" t="s">
+      <c r="C26" s="31"/>
+      <c r="D26" s="32"/>
+      <c r="I26" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="23"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="17"/>
+      <c r="O26" s="17"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
@@ -1653,17 +1657,17 @@
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="37"/>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
@@ -1724,15 +1728,15 @@
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="F34" s="18" t="s">
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="F34" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="G34" s="19"/>
+      <c r="G34" s="36"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
@@ -1770,13 +1774,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B2:Q2"/>
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="Q6:R6"/>
     <mergeCell ref="B34:D34"/>
     <mergeCell ref="F34:G34"/>
     <mergeCell ref="B30:J30"/>
-    <mergeCell ref="B2:P2"/>
     <mergeCell ref="I26:O26"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="O10:Q10"/>

</xml_diff>